<commit_message>
fix filter and add quickSearch Invoice
</commit_message>
<xml_diff>
--- a/web/uploadedFiles/Transaction.xlsx
+++ b/web/uploadedFiles/Transaction.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="75">
   <si>
     <t>Name Fund</t>
   </si>
@@ -237,54 +237,6 @@
   </si>
   <si>
     <t>Nhận tiền từ Vietcombank</t>
-  </si>
-  <si>
-    <t>Thu tiền mặt từ hóa đơn 9</t>
-  </si>
-  <si>
-    <t>Thu tiền mặt từ hóa đơn 10</t>
-  </si>
-  <si>
-    <t>Thu tiền mặt từ hóa đơn 11</t>
-  </si>
-  <si>
-    <t>Thu tiền mặt từ hóa đơn 12</t>
-  </si>
-  <si>
-    <t>Thu tiền mặt từ hóa đơn 13</t>
-  </si>
-  <si>
-    <t>Thu tiền mặt từ hóa đơn 14</t>
-  </si>
-  <si>
-    <t>Thu tiền mặt từ hóa đơn 15</t>
-  </si>
-  <si>
-    <t>Thu tiền mặt từ hóa đơn 16</t>
-  </si>
-  <si>
-    <t>Thu tiền mặt từ hóa đơn 17</t>
-  </si>
-  <si>
-    <t>Thu tiền mặt từ hóa đơn 18</t>
-  </si>
-  <si>
-    <t>Thu tiền mặt từ hóa đơn 19</t>
-  </si>
-  <si>
-    <t>Thu tiền mặt từ hóa đơn 20</t>
-  </si>
-  <si>
-    <t>Thu tiền mặt từ hóa đơn 21</t>
-  </si>
-  <si>
-    <t>Thu tiền mặt từ hóa đơn 1021</t>
-  </si>
-  <si>
-    <t>Thu tiền mặt từ hóa đơn 1022</t>
-  </si>
-  <si>
-    <t>Thu tiền mặt từ hóa đơn 1023</t>
   </si>
 </sst>
 </file>
@@ -329,7 +281,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="B1:L51"/>
+  <dimension ref="B1:L35"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -1417,518 +1369,6 @@
         <v>74</v>
       </c>
     </row>
-    <row r="36">
-      <c r="B36" t="s">
-        <v>10</v>
-      </c>
-      <c r="C36" t="s">
-        <v>11</v>
-      </c>
-      <c r="D36" t="n">
-        <v>385000.0</v>
-      </c>
-      <c r="E36" t="s">
-        <v>48</v>
-      </c>
-      <c r="F36" t="s">
-        <v>49</v>
-      </c>
-      <c r="G36" t="n">
-        <v>45839.0</v>
-      </c>
-      <c r="H36" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="I36" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="J36" t="s">
-        <v>13</v>
-      </c>
-      <c r="K36" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="B37" t="s">
-        <v>10</v>
-      </c>
-      <c r="C37" t="s">
-        <v>11</v>
-      </c>
-      <c r="D37" t="n">
-        <v>1540000.0</v>
-      </c>
-      <c r="E37" t="s">
-        <v>48</v>
-      </c>
-      <c r="F37" t="s">
-        <v>49</v>
-      </c>
-      <c r="G37" t="n">
-        <v>45839.0</v>
-      </c>
-      <c r="H37" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="I37" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="J37" t="s">
-        <v>13</v>
-      </c>
-      <c r="K37" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="B38" t="s">
-        <v>10</v>
-      </c>
-      <c r="C38" t="s">
-        <v>11</v>
-      </c>
-      <c r="D38" t="n">
-        <v>2310000.0</v>
-      </c>
-      <c r="E38" t="s">
-        <v>48</v>
-      </c>
-      <c r="F38" t="s">
-        <v>49</v>
-      </c>
-      <c r="G38" t="n">
-        <v>45839.0</v>
-      </c>
-      <c r="H38" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="I38" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="J38" t="s">
-        <v>13</v>
-      </c>
-      <c r="K38" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="B39" t="s">
-        <v>10</v>
-      </c>
-      <c r="C39" t="s">
-        <v>11</v>
-      </c>
-      <c r="D39" t="n">
-        <v>803000.0</v>
-      </c>
-      <c r="E39" t="s">
-        <v>48</v>
-      </c>
-      <c r="F39" t="s">
-        <v>49</v>
-      </c>
-      <c r="G39" t="n">
-        <v>45839.0</v>
-      </c>
-      <c r="H39" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="I39" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="J39" t="s">
-        <v>13</v>
-      </c>
-      <c r="K39" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="B40" t="s">
-        <v>10</v>
-      </c>
-      <c r="C40" t="s">
-        <v>11</v>
-      </c>
-      <c r="D40" t="n">
-        <v>1639000.0</v>
-      </c>
-      <c r="E40" t="s">
-        <v>48</v>
-      </c>
-      <c r="F40" t="s">
-        <v>49</v>
-      </c>
-      <c r="G40" t="n">
-        <v>45839.0</v>
-      </c>
-      <c r="H40" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="I40" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="J40" t="s">
-        <v>13</v>
-      </c>
-      <c r="K40" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="B41" t="s">
-        <v>10</v>
-      </c>
-      <c r="C41" t="s">
-        <v>11</v>
-      </c>
-      <c r="D41" t="n">
-        <v>385000.0</v>
-      </c>
-      <c r="E41" t="s">
-        <v>48</v>
-      </c>
-      <c r="F41" t="s">
-        <v>49</v>
-      </c>
-      <c r="G41" t="n">
-        <v>45839.0</v>
-      </c>
-      <c r="H41" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="I41" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="J41" t="s">
-        <v>13</v>
-      </c>
-      <c r="K41" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="B42" t="s">
-        <v>10</v>
-      </c>
-      <c r="C42" t="s">
-        <v>11</v>
-      </c>
-      <c r="D42" t="n">
-        <v>2926000.0</v>
-      </c>
-      <c r="E42" t="s">
-        <v>48</v>
-      </c>
-      <c r="F42" t="s">
-        <v>49</v>
-      </c>
-      <c r="G42" t="n">
-        <v>45839.0</v>
-      </c>
-      <c r="H42" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="I42" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="J42" t="s">
-        <v>13</v>
-      </c>
-      <c r="K42" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="B43" t="s">
-        <v>10</v>
-      </c>
-      <c r="C43" t="s">
-        <v>11</v>
-      </c>
-      <c r="D43" t="n">
-        <v>385000.0</v>
-      </c>
-      <c r="E43" t="s">
-        <v>48</v>
-      </c>
-      <c r="F43" t="s">
-        <v>49</v>
-      </c>
-      <c r="G43" t="n">
-        <v>45839.0</v>
-      </c>
-      <c r="H43" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="I43" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="J43" t="s">
-        <v>13</v>
-      </c>
-      <c r="K43" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="B44" t="s">
-        <v>10</v>
-      </c>
-      <c r="C44" t="s">
-        <v>11</v>
-      </c>
-      <c r="D44" t="n">
-        <v>418000.0</v>
-      </c>
-      <c r="E44" t="s">
-        <v>48</v>
-      </c>
-      <c r="F44" t="s">
-        <v>49</v>
-      </c>
-      <c r="G44" t="n">
-        <v>45839.0</v>
-      </c>
-      <c r="H44" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="I44" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="J44" t="s">
-        <v>13</v>
-      </c>
-      <c r="K44" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="B45" t="s">
-        <v>10</v>
-      </c>
-      <c r="C45" t="s">
-        <v>11</v>
-      </c>
-      <c r="D45" t="n">
-        <v>1672000.0</v>
-      </c>
-      <c r="E45" t="s">
-        <v>48</v>
-      </c>
-      <c r="F45" t="s">
-        <v>49</v>
-      </c>
-      <c r="G45" t="n">
-        <v>45839.0</v>
-      </c>
-      <c r="H45" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="I45" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="J45" t="s">
-        <v>13</v>
-      </c>
-      <c r="K45" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="B46" t="s">
-        <v>10</v>
-      </c>
-      <c r="C46" t="s">
-        <v>11</v>
-      </c>
-      <c r="D46" t="n">
-        <v>770000.0</v>
-      </c>
-      <c r="E46" t="s">
-        <v>48</v>
-      </c>
-      <c r="F46" t="s">
-        <v>49</v>
-      </c>
-      <c r="G46" t="n">
-        <v>45839.0</v>
-      </c>
-      <c r="H46" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="I46" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="J46" t="s">
-        <v>13</v>
-      </c>
-      <c r="K46" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="B47" t="s">
-        <v>10</v>
-      </c>
-      <c r="C47" t="s">
-        <v>11</v>
-      </c>
-      <c r="D47" t="n">
-        <v>418000.0</v>
-      </c>
-      <c r="E47" t="s">
-        <v>48</v>
-      </c>
-      <c r="F47" t="s">
-        <v>49</v>
-      </c>
-      <c r="G47" t="n">
-        <v>45839.0</v>
-      </c>
-      <c r="H47" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="I47" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="J47" t="s">
-        <v>13</v>
-      </c>
-      <c r="K47" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="B48" t="s">
-        <v>10</v>
-      </c>
-      <c r="C48" t="s">
-        <v>11</v>
-      </c>
-      <c r="D48" t="n">
-        <v>385000.0</v>
-      </c>
-      <c r="E48" t="s">
-        <v>48</v>
-      </c>
-      <c r="F48" t="s">
-        <v>49</v>
-      </c>
-      <c r="G48" t="n">
-        <v>45840.0</v>
-      </c>
-      <c r="H48" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="I48" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="J48" t="s">
-        <v>13</v>
-      </c>
-      <c r="K48" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="B49" t="s">
-        <v>10</v>
-      </c>
-      <c r="C49" t="s">
-        <v>11</v>
-      </c>
-      <c r="D49" t="n">
-        <v>385000.0</v>
-      </c>
-      <c r="E49" t="s">
-        <v>48</v>
-      </c>
-      <c r="F49" t="s">
-        <v>49</v>
-      </c>
-      <c r="G49" t="n">
-        <v>45840.0</v>
-      </c>
-      <c r="H49" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="I49" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="J49" t="s">
-        <v>13</v>
-      </c>
-      <c r="K49" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="B50" t="s">
-        <v>10</v>
-      </c>
-      <c r="C50" t="s">
-        <v>11</v>
-      </c>
-      <c r="D50" t="n">
-        <v>418000.0</v>
-      </c>
-      <c r="E50" t="s">
-        <v>48</v>
-      </c>
-      <c r="F50" t="s">
-        <v>49</v>
-      </c>
-      <c r="G50" t="n">
-        <v>45840.0</v>
-      </c>
-      <c r="H50" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="I50" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="J50" t="s">
-        <v>13</v>
-      </c>
-      <c r="K50" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="B51" t="s">
-        <v>10</v>
-      </c>
-      <c r="C51" t="s">
-        <v>11</v>
-      </c>
-      <c r="D51" t="n">
-        <v>385000.0</v>
-      </c>
-      <c r="E51" t="s">
-        <v>48</v>
-      </c>
-      <c r="F51" t="s">
-        <v>49</v>
-      </c>
-      <c r="G51" t="n">
-        <v>45840.0</v>
-      </c>
-      <c r="H51" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="I51" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="J51" t="s">
-        <v>13</v>
-      </c>
-      <c r="K51" t="s">
-        <v>90</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>